<commit_message>
SSP description added to SVD for ESila, VE8, VK014
</commit_message>
<xml_diff>
--- a/SVD_Files/SPI.xlsx
+++ b/SVD_Files/SPI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="183">
   <si>
     <t>Addr Shift</t>
   </si>
@@ -608,6 +608,45 @@
   </si>
   <si>
     <t>TBSYMIS</t>
+  </si>
+  <si>
+    <t>1986VE8</t>
+  </si>
+  <si>
+    <t>1923VK014</t>
+  </si>
+  <si>
+    <t>Esila</t>
+  </si>
+  <si>
+    <t>0x4008_9000</t>
+  </si>
+  <si>
+    <t>SSP5</t>
+  </si>
+  <si>
+    <t>SSP6</t>
+  </si>
+  <si>
+    <t>0x4009_5000</t>
+  </si>
+  <si>
+    <t>0x4008_A000</t>
+  </si>
+  <si>
+    <t>0x4009_6000</t>
+  </si>
+  <si>
+    <t>0x4009_7000</t>
+  </si>
+  <si>
+    <t>0x4009_8000</t>
+  </si>
+  <si>
+    <t>0x400B_1000</t>
+  </si>
+  <si>
+    <t>0x400B_2000</t>
   </si>
 </sst>
 </file>
@@ -1017,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,6 +1610,111 @@
       </c>
       <c r="K18" s="6"/>
     </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -1581,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>